<commit_message>
UDATED DATASET to add columns for assessing modulators
</commit_message>
<xml_diff>
--- a/data/df_taxa_fig.xlsx
+++ b/data/df_taxa_fig.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\Desktop\PhD_Fuster-Calvo\BiodivDatasetRetrieval\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\Desktop\PhD_Fuster-Calvo\automated_dataset_retrieval\automated_datset_retrieval\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="25476" windowHeight="15300"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="25470" windowHeight="15300"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="190">
   <si>
     <t>url</t>
   </si>
@@ -978,21 +978,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomRight" activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>49</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>49</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>55</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>57</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>57</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>61</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>63</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>65</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>68</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>70</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>72</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>74</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>74</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>76</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>78</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>79</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>83</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>87</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>89</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>91</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>93</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>94</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>96</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>98</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>100</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>101</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>103</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>104</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>106</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>107</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>109</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>110</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>111</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>112</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>114</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>115</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>117</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>117</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>119</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>120</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>122</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>124</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="E74" t="s">
         <v>181</v>
@@ -2047,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="E75" t="s">
         <v>177</v>
@@ -2056,7 +2056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>126</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>128</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>130</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>131</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="E80" t="s">
         <v>174</v>
@@ -2127,7 +2127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="E81" t="s">
         <v>182</v>
@@ -2136,7 +2136,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>133</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>135</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>137</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>139</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>141</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>143</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>145</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>147</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>148</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>150</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>152</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>153</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>155</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>155</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>155</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>157</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>159</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>161</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>162</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>164</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>164</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="103" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>166</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="104" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>168</v>
       </c>
@@ -2453,6 +2453,34 @@
       </c>
       <c r="D104" s="1" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>49</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E105" t="s">
+        <v>181</v>
+      </c>
+      <c r="F105">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>49</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E106" t="s">
+        <v>177</v>
+      </c>
+      <c r="F106">
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>